<commit_message>
push latihan 4 Contoh CRC Card
</commit_message>
<xml_diff>
--- a/minggu-1/02/contoh CRC card.xlsx
+++ b/minggu-1/02/contoh CRC card.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\to-DO\praxis-academy\minggu-1\02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\praxis-academy\minggu-1\02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C1C852-3F9E-42CD-AF82-B5DEC35CDD72}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61C0D70-996C-4E28-911F-DB7D8B8FE095}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67229D71-84C5-4BFB-8EC4-0B8899EBB84F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="16">
   <si>
     <t>Class</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>staff</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -295,52 +298,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -358,6 +361,173 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ED573AE-D15A-4BDD-878B-836D51938A8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="847725"/>
+          <a:ext cx="0" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A0B5003-8C00-4D7C-9F21-622984996A61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190875" y="438150"/>
+          <a:ext cx="1647825" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF106C01-BB91-42F6-96F6-EC181935ED23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3086100" y="1638300"/>
+          <a:ext cx="1905000" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A377AC7-D677-4B09-9751-C622C872C5E8}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,136 +843,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+      <c r="J5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="1" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="E6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="2"/>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="8"/>
+      <c r="K6" s="11"/>
       <c r="L6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="10"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="3" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="2" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>